<commit_message>
Excel template & com ports .Txt updated.
</commit_message>
<xml_diff>
--- a/serPort/Test Template.xlsx
+++ b/serPort/Test Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\serPort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{45EE2B9B-ED37-494F-AB1E-2A704488B2E8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{07E8430C-F52E-44B2-AD82-27520FA45231}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="9480" xr2:uid="{E0978ADF-A891-4F84-A2D4-3883FD4436BC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>Sto at:</t>
   </si>
@@ -40,6 +40,48 @@
   </si>
   <si>
     <t>Hysteresis:</t>
+  </si>
+  <si>
+    <t>Mitutoyo 1</t>
+  </si>
+  <si>
+    <t>Operator:</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Huber ID:</t>
+  </si>
+  <si>
+    <t>Check Type:</t>
+  </si>
+  <si>
+    <t>Start t:</t>
+  </si>
+  <si>
+    <t>Stop t:</t>
+  </si>
+  <si>
+    <t>Data Res.:</t>
+  </si>
+  <si>
+    <t>Start time:</t>
+  </si>
+  <si>
+    <t>Stop time:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sended to: </t>
+  </si>
+  <si>
+    <t>Doc. Name:</t>
+  </si>
+  <si>
+    <t>Therm. Type:</t>
+  </si>
+  <si>
+    <t>Mitutoyo 2</t>
   </si>
 </sst>
 </file>
@@ -56,15 +98,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -72,12 +120,134 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,43 +562,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B4E1BB-4251-4B37-B59B-FE59E82EE140}">
-  <dimension ref="E2:E6"/>
+  <dimension ref="D1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:5">
-      <c r="E2" t="s">
+    <row r="1" spans="4:11">
+      <c r="D1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="J1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="11"/>
+    </row>
+    <row r="2" spans="4:11">
+      <c r="D2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="J2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="4:11">
+      <c r="D3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="J3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="4:11">
+      <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="5:5">
-      <c r="E3" t="s">
+      <c r="E4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="4:11">
+      <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="5:5">
-      <c r="E4" t="s">
+      <c r="E5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="4:11">
+      <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="5:5">
-      <c r="E5" t="s">
+      <c r="E6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="4:11">
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="5:5">
-      <c r="E6" t="s">
+      <c r="E7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="4:11">
+      <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="4:11">
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="J9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="4:11">
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="J10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="4:11">
+      <c r="D11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="J11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="4:11">
+      <c r="D12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="J12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="4:11">
+      <c r="D13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="J13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="4:11">
+      <c r="D14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="J14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="4:11">
+      <c r="D15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="J15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="4:11">
+      <c r="D16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="J16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="4:11">
+      <c r="D17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="J17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="4:11">
+      <c r="D18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="J18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Version 0.2.01 (Alpha) - Two Indicators & Only UP (Rate 1).
</commit_message>
<xml_diff>
--- a/serPort/Test Template.xlsx
+++ b/serPort/Test Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\serPort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{07E8430C-F52E-44B2-AD82-27520FA45231}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E1775312-932C-4C9F-B5CE-8AF849EC1964}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="9480" xr2:uid="{E0978ADF-A891-4F84-A2D4-3883FD4436BC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>Sto at:</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Mitutoyo 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Captured Val: </t>
   </si>
 </sst>
 </file>
@@ -562,202 +565,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B4E1BB-4251-4B37-B59B-FE59E82EE140}">
-  <dimension ref="D1:K18"/>
+  <dimension ref="D1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:11">
+    <row r="1" spans="4:10">
       <c r="D1" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="11"/>
-      <c r="J1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="11"/>
-    </row>
-    <row r="2" spans="4:11">
+      <c r="J1" s="11"/>
+    </row>
+    <row r="2" spans="4:10">
       <c r="D2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="4:11">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="4:10">
       <c r="D3" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="J3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="4:11">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="4:10">
       <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="J4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="4:11">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="4:10">
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="J5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="4:11">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="4:10">
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="J6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="4:11">
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="4:10">
       <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="J7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="4:11">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="4:10">
       <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="J8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="4:11">
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="4:10">
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="J9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="4:11">
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="4:10">
       <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="J10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="4:11">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="4:10">
       <c r="D11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="J11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="4:11">
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="4:10">
       <c r="D12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="J12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="4:11">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="4:10">
       <c r="D13" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="J13" s="6" t="s">
+      <c r="I13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="4:11">
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="4:10">
       <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="J14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="4:11">
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="4:10">
       <c r="D15" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="J15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="4:11">
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="4:10">
       <c r="D16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="J16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="4:11">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="4:10">
       <c r="D17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="J17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="4:11">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="4:10">
       <c r="D18" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="7"/>
-      <c r="J18" s="6" t="s">
+      <c r="I18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K18" s="7"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="4:10">
+      <c r="D19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="I19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>